<commit_message>
Added HUF, EURHUF, EURRON, ERPLN, EURCZK
</commit_message>
<xml_diff>
--- a/Descriptive.xlsx
+++ b/Descriptive.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="34">
   <si>
     <t>Mean</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>MXN Curncy</t>
+  </si>
+  <si>
+    <t>HUF Curncy</t>
+  </si>
+  <si>
+    <t>EURHUF Curncy</t>
+  </si>
+  <si>
+    <t>EURCZK Curncy</t>
+  </si>
+  <si>
+    <t>EURPLN Curncy</t>
+  </si>
+  <si>
+    <t>EURRON Curncy</t>
   </si>
 </sst>
 </file>
@@ -460,7 +475,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -963,6 +978,106 @@
         <v>10.77803299867064</v>
       </c>
     </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>0.02363195930922908</v>
+      </c>
+      <c r="C26">
+        <v>0.6377919836678589</v>
+      </c>
+      <c r="D26">
+        <v>4.0647161170311e-05</v>
+      </c>
+      <c r="E26">
+        <v>0.1509486154187198</v>
+      </c>
+      <c r="F26">
+        <v>1.68478710996819</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>0.007787567288197178</v>
+      </c>
+      <c r="C27">
+        <v>0.3463469130889365</v>
+      </c>
+      <c r="D27">
+        <v>1.198656512370231e-05</v>
+      </c>
+      <c r="E27">
+        <v>0.03411258613253276</v>
+      </c>
+      <c r="F27">
+        <v>1.801818390454927</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>0.0007229347639865785</v>
+      </c>
+      <c r="C28">
+        <v>0.2159393934443844</v>
+      </c>
+      <c r="D28">
+        <v>4.659462932290892e-06</v>
+      </c>
+      <c r="E28">
+        <v>6.835627131305123</v>
+      </c>
+      <c r="F28">
+        <v>158.0163496588241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0.002717643720726279</v>
+      </c>
+      <c r="C29">
+        <v>0.3651904477642741</v>
+      </c>
+      <c r="D29">
+        <v>1.332634110151478e-05</v>
+      </c>
+      <c r="E29">
+        <v>0.2205079774657492</v>
+      </c>
+      <c r="F29">
+        <v>2.281371321679849</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>0.003905218945769118</v>
+      </c>
+      <c r="C30">
+        <v>0.1866110436219047</v>
+      </c>
+      <c r="D30">
+        <v>3.479739957780611e-06</v>
+      </c>
+      <c r="E30">
+        <v>0.4246326835344242</v>
+      </c>
+      <c r="F30">
+        <v>3.686317955200333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -970,13 +1085,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AD30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1049,8 +1164,23 @@
       <c r="Y1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Z1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1126,8 +1256,23 @@
       <c r="Y2">
         <v>0.0515880760591212</v>
       </c>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="Z2">
+        <v>0.06081490950031013</v>
+      </c>
+      <c r="AA2">
+        <v>0.01119252915668114</v>
+      </c>
+      <c r="AB2">
+        <v>0.005209991548572055</v>
+      </c>
+      <c r="AC2">
+        <v>0.01621724230875039</v>
+      </c>
+      <c r="AD2">
+        <v>0.003036095106320619</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1203,8 +1348,23 @@
       <c r="Y3">
         <v>0.1126666860263633</v>
       </c>
-    </row>
-    <row r="4" spans="1:25">
+      <c r="Z3">
+        <v>0.2988134206485495</v>
+      </c>
+      <c r="AA3">
+        <v>0.01641711538974513</v>
+      </c>
+      <c r="AB3">
+        <v>0.05179597315355735</v>
+      </c>
+      <c r="AC3">
+        <v>0.01351259231365778</v>
+      </c>
+      <c r="AD3">
+        <v>0.004558236981023895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1280,8 +1440,23 @@
       <c r="Y4">
         <v>-0.09556067064135138</v>
       </c>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="Z4">
+        <v>-0.2822516817732626</v>
+      </c>
+      <c r="AA4">
+        <v>-0.005427179904188177</v>
+      </c>
+      <c r="AB4">
+        <v>-0.005171851901587081</v>
+      </c>
+      <c r="AC4">
+        <v>0.001247912588026183</v>
+      </c>
+      <c r="AD4">
+        <v>-6.685660565577167e-05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1357,8 +1532,23 @@
       <c r="Y5">
         <v>0.1978278507852778</v>
       </c>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="Z5">
+        <v>0.3487901588682131</v>
+      </c>
+      <c r="AA5">
+        <v>0.07354700405196986</v>
+      </c>
+      <c r="AB5">
+        <v>0.0199968289119543</v>
+      </c>
+      <c r="AC5">
+        <v>0.1329051880156559</v>
+      </c>
+      <c r="AD5">
+        <v>0.01450648675884704</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1434,8 +1624,23 @@
       <c r="Y6">
         <v>0.10944210973968</v>
       </c>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="Z6">
+        <v>0.2902867099989758</v>
+      </c>
+      <c r="AA6">
+        <v>0.01651975634020541</v>
+      </c>
+      <c r="AB6">
+        <v>0.009338172246966446</v>
+      </c>
+      <c r="AC6">
+        <v>0.01292106947195684</v>
+      </c>
+      <c r="AD6">
+        <v>0.03141933208129765</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1511,8 +1716,23 @@
       <c r="Y7">
         <v>0.3179236781207332</v>
       </c>
-    </row>
-    <row r="8" spans="1:25">
+      <c r="Z7">
+        <v>0.12691916128414</v>
+      </c>
+      <c r="AA7">
+        <v>0.08601599013708322</v>
+      </c>
+      <c r="AB7">
+        <v>0.0144289536459897</v>
+      </c>
+      <c r="AC7">
+        <v>0.09926977339436931</v>
+      </c>
+      <c r="AD7">
+        <v>0.02221406798563754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1588,8 +1808,23 @@
       <c r="Y8">
         <v>0.1118208526225566</v>
       </c>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="Z8">
+        <v>0.1249109042224111</v>
+      </c>
+      <c r="AA8">
+        <v>0.02126098595944997</v>
+      </c>
+      <c r="AB8">
+        <v>0.004683109134683643</v>
+      </c>
+      <c r="AC8">
+        <v>0.02594329778048064</v>
+      </c>
+      <c r="AD8">
+        <v>0.00605127111186011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1665,8 +1900,23 @@
       <c r="Y9">
         <v>0.3183115855301107</v>
       </c>
-    </row>
-    <row r="10" spans="1:25">
+      <c r="Z9">
+        <v>0.2263297298015128</v>
+      </c>
+      <c r="AA9">
+        <v>0.09459847458009009</v>
+      </c>
+      <c r="AB9">
+        <v>0.01270259792077918</v>
+      </c>
+      <c r="AC9">
+        <v>0.0915017732455225</v>
+      </c>
+      <c r="AD9">
+        <v>0.02046841253111412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1742,8 +1992,23 @@
       <c r="Y10">
         <v>-0.09556067064135138</v>
       </c>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="Z10">
+        <v>-0.2822516817732626</v>
+      </c>
+      <c r="AA10">
+        <v>-0.005427179904188177</v>
+      </c>
+      <c r="AB10">
+        <v>-0.005171851901587081</v>
+      </c>
+      <c r="AC10">
+        <v>0.001247912588026183</v>
+      </c>
+      <c r="AD10">
+        <v>-6.685660565577167e-05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1819,8 +2084,23 @@
       <c r="Y11">
         <v>0.457296906580707</v>
       </c>
-    </row>
-    <row r="12" spans="1:25">
+      <c r="Z11">
+        <v>0.2965012026482508</v>
+      </c>
+      <c r="AA11">
+        <v>0.1246031627827413</v>
+      </c>
+      <c r="AB11">
+        <v>0.02183427127210451</v>
+      </c>
+      <c r="AC11">
+        <v>0.1425087983449788</v>
+      </c>
+      <c r="AD11">
+        <v>0.02650748075239313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1896,8 +2176,23 @@
       <c r="Y12">
         <v>0.08947809818389274</v>
       </c>
-    </row>
-    <row r="13" spans="1:25">
+      <c r="Z12">
+        <v>0.08142491719299347</v>
+      </c>
+      <c r="AA12">
+        <v>0.04050373807735004</v>
+      </c>
+      <c r="AB12">
+        <v>0.001341852527576867</v>
+      </c>
+      <c r="AC12">
+        <v>0.02688046805827636</v>
+      </c>
+      <c r="AD12">
+        <v>0.003994122562744605</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1973,8 +2268,23 @@
       <c r="Y13">
         <v>0.3796756597400969</v>
       </c>
-    </row>
-    <row r="14" spans="1:25">
+      <c r="Z13">
+        <v>0.1897980901385529</v>
+      </c>
+      <c r="AA13">
+        <v>0.08548604614802181</v>
+      </c>
+      <c r="AB13">
+        <v>0.0179414954290666</v>
+      </c>
+      <c r="AC13">
+        <v>0.0916847504155229</v>
+      </c>
+      <c r="AD13">
+        <v>0.02146945131445341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -2050,8 +2360,23 @@
       <c r="Y14">
         <v>0.1826274958181474</v>
       </c>
-    </row>
-    <row r="15" spans="1:25">
+      <c r="Z14">
+        <v>0.1122735126544697</v>
+      </c>
+      <c r="AA14">
+        <v>0.04723643430975753</v>
+      </c>
+      <c r="AB14">
+        <v>0.010159556761568</v>
+      </c>
+      <c r="AC14">
+        <v>0.05251546413481828</v>
+      </c>
+      <c r="AD14">
+        <v>0.01127174684701565</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2127,8 +2452,23 @@
       <c r="Y15">
         <v>0.01924111715527721</v>
       </c>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="Z15">
+        <v>0.02912139129853841</v>
+      </c>
+      <c r="AA15">
+        <v>0.005944123317570492</v>
+      </c>
+      <c r="AB15">
+        <v>0.003624000659074894</v>
+      </c>
+      <c r="AC15">
+        <v>0.008996107903615621</v>
+      </c>
+      <c r="AD15">
+        <v>0.0009913807619272065</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2204,8 +2544,23 @@
       <c r="Y16">
         <v>0.2944272374238037</v>
       </c>
-    </row>
-    <row r="17" spans="1:25">
+      <c r="Z16">
+        <v>0.1283096925339937</v>
+      </c>
+      <c r="AA16">
+        <v>0.05344818649039693</v>
+      </c>
+      <c r="AB16">
+        <v>0.01445776569898406</v>
+      </c>
+      <c r="AC16">
+        <v>0.07669942090625326</v>
+      </c>
+      <c r="AD16">
+        <v>0.01279076939854604</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -2281,8 +2636,23 @@
       <c r="Y17">
         <v>0.01648908210108771</v>
       </c>
-    </row>
-    <row r="18" spans="1:25">
+      <c r="Z17">
+        <v>0.01984342153674231</v>
+      </c>
+      <c r="AA17">
+        <v>0.01134356678595258</v>
+      </c>
+      <c r="AB17">
+        <v>0.001856494998164766</v>
+      </c>
+      <c r="AC17">
+        <v>0.01692615104245383</v>
+      </c>
+      <c r="AD17">
+        <v>0.005015397808112637</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -2358,8 +2728,23 @@
       <c r="Y18">
         <v>0.03535219563640504</v>
       </c>
-    </row>
-    <row r="19" spans="1:25">
+      <c r="Z18">
+        <v>0.0224352620375268</v>
+      </c>
+      <c r="AA18">
+        <v>0.01712921696956131</v>
+      </c>
+      <c r="AB18">
+        <v>0.005389367343978465</v>
+      </c>
+      <c r="AC18">
+        <v>0.02721730420360182</v>
+      </c>
+      <c r="AD18">
+        <v>0.005460004745436097</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -2435,8 +2820,23 @@
       <c r="Y19">
         <v>0.04407330142928829</v>
       </c>
-    </row>
-    <row r="20" spans="1:25">
+      <c r="Z19">
+        <v>0.03343825947225401</v>
+      </c>
+      <c r="AA19">
+        <v>0.01811315985229882</v>
+      </c>
+      <c r="AB19">
+        <v>0.00199121554533669</v>
+      </c>
+      <c r="AC19">
+        <v>0.02716937093581642</v>
+      </c>
+      <c r="AD19">
+        <v>0.004929539951242353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -2512,8 +2912,23 @@
       <c r="Y20">
         <v>0.04902973567160201</v>
       </c>
-    </row>
-    <row r="21" spans="1:25">
+      <c r="Z20">
+        <v>0.02657003406288198</v>
+      </c>
+      <c r="AA20">
+        <v>0.01499913823853303</v>
+      </c>
+      <c r="AB20">
+        <v>0.003472135883545384</v>
+      </c>
+      <c r="AC20">
+        <v>0.02089810033032732</v>
+      </c>
+      <c r="AD20">
+        <v>0.00709863774417091</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -2589,8 +3004,23 @@
       <c r="Y21">
         <v>0.08105643474040662</v>
       </c>
-    </row>
-    <row r="22" spans="1:25">
+      <c r="Z21">
+        <v>0.04714285945951628</v>
+      </c>
+      <c r="AA21">
+        <v>0.01867486300071499</v>
+      </c>
+      <c r="AB21">
+        <v>0.003471840702375512</v>
+      </c>
+      <c r="AC21">
+        <v>0.02304747246647686</v>
+      </c>
+      <c r="AD21">
+        <v>0.002896523136282982</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2666,8 +3096,23 @@
       <c r="Y22">
         <v>0.0107894492741144</v>
       </c>
-    </row>
-    <row r="23" spans="1:25">
+      <c r="Z22">
+        <v>0.01335022800497521</v>
+      </c>
+      <c r="AA22">
+        <v>0.009027940024461981</v>
+      </c>
+      <c r="AB22">
+        <v>0.00276356567855059</v>
+      </c>
+      <c r="AC22">
+        <v>0.009824089741919909</v>
+      </c>
+      <c r="AD22">
+        <v>0.001786625717723236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -2743,8 +3188,23 @@
       <c r="Y23">
         <v>0.01875674842351723</v>
       </c>
-    </row>
-    <row r="24" spans="1:25">
+      <c r="Z23">
+        <v>0.02664671250550031</v>
+      </c>
+      <c r="AA23">
+        <v>0.01015696500220907</v>
+      </c>
+      <c r="AB23">
+        <v>0.002819084248698387</v>
+      </c>
+      <c r="AC23">
+        <v>0.01176610669299555</v>
+      </c>
+      <c r="AD23">
+        <v>0.003873785906844395</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -2820,8 +3280,23 @@
       <c r="Y24">
         <v>0.01403114041569592</v>
       </c>
-    </row>
-    <row r="25" spans="1:25">
+      <c r="Z24">
+        <v>0.008092648858283953</v>
+      </c>
+      <c r="AA24">
+        <v>0.006721159303239238</v>
+      </c>
+      <c r="AB24">
+        <v>0.002017913278992799</v>
+      </c>
+      <c r="AC24">
+        <v>0.01378276541176098</v>
+      </c>
+      <c r="AD24">
+        <v>0.002200717084995738</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -2896,6 +3371,481 @@
       </c>
       <c r="Y25">
         <v>0.5971909731428644</v>
+      </c>
+      <c r="Z25">
+        <v>0.1774195814984032</v>
+      </c>
+      <c r="AA25">
+        <v>0.08173911350553348</v>
+      </c>
+      <c r="AB25">
+        <v>0.01647724382673729</v>
+      </c>
+      <c r="AC25">
+        <v>0.1012381177935343</v>
+      </c>
+      <c r="AD25">
+        <v>0.01460449084928216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>0.06081490950031013</v>
+      </c>
+      <c r="C26">
+        <v>0.2988134206485495</v>
+      </c>
+      <c r="D26">
+        <v>-0.2822516817732626</v>
+      </c>
+      <c r="E26">
+        <v>0.3487901588682131</v>
+      </c>
+      <c r="F26">
+        <v>0.2902867099989758</v>
+      </c>
+      <c r="G26">
+        <v>0.12691916128414</v>
+      </c>
+      <c r="H26">
+        <v>0.1249109042224111</v>
+      </c>
+      <c r="I26">
+        <v>0.2263297298015128</v>
+      </c>
+      <c r="J26">
+        <v>-0.2822516817732626</v>
+      </c>
+      <c r="K26">
+        <v>0.2965012026482508</v>
+      </c>
+      <c r="L26">
+        <v>0.08142491719299347</v>
+      </c>
+      <c r="M26">
+        <v>0.1897980901385529</v>
+      </c>
+      <c r="N26">
+        <v>0.1122735126544697</v>
+      </c>
+      <c r="O26">
+        <v>0.02912139129853841</v>
+      </c>
+      <c r="P26">
+        <v>0.1283096925339937</v>
+      </c>
+      <c r="Q26">
+        <v>0.01984342153674231</v>
+      </c>
+      <c r="R26">
+        <v>0.0224352620375268</v>
+      </c>
+      <c r="S26">
+        <v>0.03343825947225401</v>
+      </c>
+      <c r="T26">
+        <v>0.02657003406288198</v>
+      </c>
+      <c r="U26">
+        <v>0.04714285945951628</v>
+      </c>
+      <c r="V26">
+        <v>0.01335022800497521</v>
+      </c>
+      <c r="W26">
+        <v>0.02664671250550031</v>
+      </c>
+      <c r="X26">
+        <v>0.008092648858283953</v>
+      </c>
+      <c r="Y26">
+        <v>0.1774195814984032</v>
+      </c>
+      <c r="Z26">
+        <v>0.406778614430983</v>
+      </c>
+      <c r="AA26">
+        <v>0.1246945069169128</v>
+      </c>
+      <c r="AB26">
+        <v>0.01591887995568768</v>
+      </c>
+      <c r="AC26">
+        <v>0.06724824033525174</v>
+      </c>
+      <c r="AD26">
+        <v>0.01153116934781488</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>0.01119252915668114</v>
+      </c>
+      <c r="C27">
+        <v>0.01641711538974513</v>
+      </c>
+      <c r="D27">
+        <v>-0.005427179904188177</v>
+      </c>
+      <c r="E27">
+        <v>0.07354700405196986</v>
+      </c>
+      <c r="F27">
+        <v>0.01651975634020541</v>
+      </c>
+      <c r="G27">
+        <v>0.08601599013708322</v>
+      </c>
+      <c r="H27">
+        <v>0.02126098595944997</v>
+      </c>
+      <c r="I27">
+        <v>0.09459847458009009</v>
+      </c>
+      <c r="J27">
+        <v>-0.005427179904188177</v>
+      </c>
+      <c r="K27">
+        <v>0.1246031627827413</v>
+      </c>
+      <c r="L27">
+        <v>0.04050373807735004</v>
+      </c>
+      <c r="M27">
+        <v>0.08548604614802181</v>
+      </c>
+      <c r="N27">
+        <v>0.04723643430975753</v>
+      </c>
+      <c r="O27">
+        <v>0.005944123317570492</v>
+      </c>
+      <c r="P27">
+        <v>0.05344818649039693</v>
+      </c>
+      <c r="Q27">
+        <v>0.01134356678595258</v>
+      </c>
+      <c r="R27">
+        <v>0.01712921696956131</v>
+      </c>
+      <c r="S27">
+        <v>0.01811315985229882</v>
+      </c>
+      <c r="T27">
+        <v>0.01499913823853303</v>
+      </c>
+      <c r="U27">
+        <v>0.01867486300071499</v>
+      </c>
+      <c r="V27">
+        <v>0.009027940024461981</v>
+      </c>
+      <c r="W27">
+        <v>0.01015696500220907</v>
+      </c>
+      <c r="X27">
+        <v>0.006721159303239238</v>
+      </c>
+      <c r="Y27">
+        <v>0.08173911350553348</v>
+      </c>
+      <c r="Z27">
+        <v>0.1246945069169128</v>
+      </c>
+      <c r="AA27">
+        <v>0.1199561842062356</v>
+      </c>
+      <c r="AB27">
+        <v>0.01088234458021607</v>
+      </c>
+      <c r="AC27">
+        <v>0.06810468336725482</v>
+      </c>
+      <c r="AD27">
+        <v>0.01148000044815977</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>0.005209991548572055</v>
+      </c>
+      <c r="C28">
+        <v>0.05179597315355735</v>
+      </c>
+      <c r="D28">
+        <v>-0.005171851901587081</v>
+      </c>
+      <c r="E28">
+        <v>0.0199968289119543</v>
+      </c>
+      <c r="F28">
+        <v>0.009338172246966446</v>
+      </c>
+      <c r="G28">
+        <v>0.0144289536459897</v>
+      </c>
+      <c r="H28">
+        <v>0.004683109134683643</v>
+      </c>
+      <c r="I28">
+        <v>0.01270259792077918</v>
+      </c>
+      <c r="J28">
+        <v>-0.005171851901587081</v>
+      </c>
+      <c r="K28">
+        <v>0.02183427127210451</v>
+      </c>
+      <c r="L28">
+        <v>0.001341852527576867</v>
+      </c>
+      <c r="M28">
+        <v>0.0179414954290666</v>
+      </c>
+      <c r="N28">
+        <v>0.010159556761568</v>
+      </c>
+      <c r="O28">
+        <v>0.003624000659074894</v>
+      </c>
+      <c r="P28">
+        <v>0.01445776569898406</v>
+      </c>
+      <c r="Q28">
+        <v>0.001856494998164766</v>
+      </c>
+      <c r="R28">
+        <v>0.005389367343978465</v>
+      </c>
+      <c r="S28">
+        <v>0.00199121554533669</v>
+      </c>
+      <c r="T28">
+        <v>0.003472135883545384</v>
+      </c>
+      <c r="U28">
+        <v>0.003471840702375512</v>
+      </c>
+      <c r="V28">
+        <v>0.00276356567855059</v>
+      </c>
+      <c r="W28">
+        <v>0.002819084248698387</v>
+      </c>
+      <c r="X28">
+        <v>0.002017913278992799</v>
+      </c>
+      <c r="Y28">
+        <v>0.01647724382673729</v>
+      </c>
+      <c r="Z28">
+        <v>0.01591887995568768</v>
+      </c>
+      <c r="AA28">
+        <v>0.01088234458021607</v>
+      </c>
+      <c r="AB28">
+        <v>0.04662982164112876</v>
+      </c>
+      <c r="AC28">
+        <v>0.01468984634752158</v>
+      </c>
+      <c r="AD28">
+        <v>0.004463939730030114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0.01621724230875039</v>
+      </c>
+      <c r="C29">
+        <v>0.01351259231365778</v>
+      </c>
+      <c r="D29">
+        <v>0.001247912588026183</v>
+      </c>
+      <c r="E29">
+        <v>0.1329051880156559</v>
+      </c>
+      <c r="F29">
+        <v>0.01292106947195684</v>
+      </c>
+      <c r="G29">
+        <v>0.09926977339436931</v>
+      </c>
+      <c r="H29">
+        <v>0.02594329778048064</v>
+      </c>
+      <c r="I29">
+        <v>0.0915017732455225</v>
+      </c>
+      <c r="J29">
+        <v>0.001247912588026183</v>
+      </c>
+      <c r="K29">
+        <v>0.1425087983449788</v>
+      </c>
+      <c r="L29">
+        <v>0.02688046805827636</v>
+      </c>
+      <c r="M29">
+        <v>0.0916847504155229</v>
+      </c>
+      <c r="N29">
+        <v>0.05251546413481828</v>
+      </c>
+      <c r="O29">
+        <v>0.008996107903615621</v>
+      </c>
+      <c r="P29">
+        <v>0.07669942090625326</v>
+      </c>
+      <c r="Q29">
+        <v>0.01692615104245383</v>
+      </c>
+      <c r="R29">
+        <v>0.02721730420360182</v>
+      </c>
+      <c r="S29">
+        <v>0.02716937093581642</v>
+      </c>
+      <c r="T29">
+        <v>0.02089810033032732</v>
+      </c>
+      <c r="U29">
+        <v>0.02304747246647686</v>
+      </c>
+      <c r="V29">
+        <v>0.009824089741919909</v>
+      </c>
+      <c r="W29">
+        <v>0.01176610669299555</v>
+      </c>
+      <c r="X29">
+        <v>0.01378276541176098</v>
+      </c>
+      <c r="Y29">
+        <v>0.1012381177935343</v>
+      </c>
+      <c r="Z29">
+        <v>0.06724824033525174</v>
+      </c>
+      <c r="AA29">
+        <v>0.06810468336725482</v>
+      </c>
+      <c r="AB29">
+        <v>0.01468984634752158</v>
+      </c>
+      <c r="AC29">
+        <v>0.1333640631382711</v>
+      </c>
+      <c r="AD29">
+        <v>0.01397760432527236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>0.003036095106320619</v>
+      </c>
+      <c r="C30">
+        <v>0.004558236981023895</v>
+      </c>
+      <c r="D30">
+        <v>-6.685660565577167e-05</v>
+      </c>
+      <c r="E30">
+        <v>0.01450648675884704</v>
+      </c>
+      <c r="F30">
+        <v>0.03141933208129765</v>
+      </c>
+      <c r="G30">
+        <v>0.02221406798563754</v>
+      </c>
+      <c r="H30">
+        <v>0.00605127111186011</v>
+      </c>
+      <c r="I30">
+        <v>0.02046841253111412</v>
+      </c>
+      <c r="J30">
+        <v>-6.685660565577167e-05</v>
+      </c>
+      <c r="K30">
+        <v>0.02650748075239313</v>
+      </c>
+      <c r="L30">
+        <v>0.003994122562744605</v>
+      </c>
+      <c r="M30">
+        <v>0.02146945131445341</v>
+      </c>
+      <c r="N30">
+        <v>0.01127174684701565</v>
+      </c>
+      <c r="O30">
+        <v>0.0009913807619272065</v>
+      </c>
+      <c r="P30">
+        <v>0.01279076939854604</v>
+      </c>
+      <c r="Q30">
+        <v>0.005015397808112637</v>
+      </c>
+      <c r="R30">
+        <v>0.005460004745436097</v>
+      </c>
+      <c r="S30">
+        <v>0.004929539951242353</v>
+      </c>
+      <c r="T30">
+        <v>0.00709863774417091</v>
+      </c>
+      <c r="U30">
+        <v>0.002896523136282982</v>
+      </c>
+      <c r="V30">
+        <v>0.001786625717723236</v>
+      </c>
+      <c r="W30">
+        <v>0.003873785906844395</v>
+      </c>
+      <c r="X30">
+        <v>0.002200717084995738</v>
+      </c>
+      <c r="Y30">
+        <v>0.01460449084928216</v>
+      </c>
+      <c r="Z30">
+        <v>0.01153116934781488</v>
+      </c>
+      <c r="AA30">
+        <v>0.01148000044815977</v>
+      </c>
+      <c r="AB30">
+        <v>0.004463939730030114</v>
+      </c>
+      <c r="AC30">
+        <v>0.01397760432527236</v>
+      </c>
+      <c r="AD30">
+        <v>0.03482368160165643</v>
       </c>
     </row>
   </sheetData>
@@ -2905,13 +3855,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AD30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2984,8 +3934,23 @@
       <c r="Y1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Z1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3061,8 +4026,23 @@
       <c r="Y2">
         <v>0.2590446592134604</v>
       </c>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="Z2">
+        <v>0.3700095530544901</v>
+      </c>
+      <c r="AA2">
+        <v>0.1254003768781572</v>
+      </c>
+      <c r="AB2">
+        <v>0.09362397374024603</v>
+      </c>
+      <c r="AC2">
+        <v>0.1723215232906715</v>
+      </c>
+      <c r="AD2">
+        <v>0.0631335134076476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -3138,8 +4118,23 @@
       <c r="Y3">
         <v>0.2516668116386254</v>
       </c>
-    </row>
-    <row r="4" spans="1:25">
+      <c r="Z3">
+        <v>0.8087384417639576</v>
+      </c>
+      <c r="AA3">
+        <v>0.08182246775480589</v>
+      </c>
+      <c r="AB3">
+        <v>0.4140484508790929</v>
+      </c>
+      <c r="AC3">
+        <v>0.06387138136257922</v>
+      </c>
+      <c r="AD3">
+        <v>0.04216446582810775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -3215,8 +4210,23 @@
       <c r="Y4">
         <v>-0.2349372077103835</v>
       </c>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="Z4">
+        <v>-0.8407884033512402</v>
+      </c>
+      <c r="AA4">
+        <v>-0.02977091124346888</v>
+      </c>
+      <c r="AB4">
+        <v>-0.0455033566070495</v>
+      </c>
+      <c r="AC4">
+        <v>0.006492231348953815</v>
+      </c>
+      <c r="AD4">
+        <v>-0.0006806693777868312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -3292,8 +4302,23 @@
       <c r="Y5">
         <v>0.4004029173811289</v>
       </c>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="Z5">
+        <v>0.8553652132840053</v>
+      </c>
+      <c r="AA5">
+        <v>0.3321391598127916</v>
+      </c>
+      <c r="AB5">
+        <v>0.1448423863224391</v>
+      </c>
+      <c r="AC5">
+        <v>0.5692315229931343</v>
+      </c>
+      <c r="AD5">
+        <v>0.1215881699463247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -3369,8 +4394,23 @@
       <c r="Y6">
         <v>0.2573640526143546</v>
       </c>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="Z6">
+        <v>0.8271192801682246</v>
+      </c>
+      <c r="AA6">
+        <v>0.08667869488723651</v>
+      </c>
+      <c r="AB6">
+        <v>0.0785868806609568</v>
+      </c>
+      <c r="AC6">
+        <v>0.06429824212392583</v>
+      </c>
+      <c r="AD6">
+        <v>0.3059705690643176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -3446,8 +4486,23 @@
       <c r="Y7">
         <v>0.3115974966668293</v>
       </c>
-    </row>
-    <row r="8" spans="1:25">
+      <c r="Z7">
+        <v>0.1507217195110394</v>
+      </c>
+      <c r="AA7">
+        <v>0.1881029361635364</v>
+      </c>
+      <c r="AB7">
+        <v>0.05060933887733886</v>
+      </c>
+      <c r="AC7">
+        <v>0.2058852927497622</v>
+      </c>
+      <c r="AD7">
+        <v>0.09016094561642715</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -3523,8 +4578,23 @@
       <c r="Y8">
         <v>0.4422555951856511</v>
       </c>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="Z8">
+        <v>0.5985886114067224</v>
+      </c>
+      <c r="AA8">
+        <v>0.1876200439702971</v>
+      </c>
+      <c r="AB8">
+        <v>0.06628412924595636</v>
+      </c>
+      <c r="AC8">
+        <v>0.2171265467651519</v>
+      </c>
+      <c r="AD8">
+        <v>0.0991097596899662</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -3600,8 +4670,23 @@
       <c r="Y9">
         <v>0.3959866928779132</v>
       </c>
-    </row>
-    <row r="10" spans="1:25">
+      <c r="Z9">
+        <v>0.3411515208744616</v>
+      </c>
+      <c r="AA9">
+        <v>0.2625775400123104</v>
+      </c>
+      <c r="AB9">
+        <v>0.05655167039615811</v>
+      </c>
+      <c r="AC9">
+        <v>0.2408767397452142</v>
+      </c>
+      <c r="AD9">
+        <v>0.1054463576487062</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -3677,8 +4762,23 @@
       <c r="Y10">
         <v>-0.2349372077103835</v>
       </c>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="Z10">
+        <v>-0.8407884033512402</v>
+      </c>
+      <c r="AA10">
+        <v>-0.02977091124346888</v>
+      </c>
+      <c r="AB10">
+        <v>-0.0455033566070495</v>
+      </c>
+      <c r="AC10">
+        <v>0.006492231348953815</v>
+      </c>
+      <c r="AD10">
+        <v>-0.0006806693777868312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -3754,8 +4854,23 @@
       <c r="Y11">
         <v>0.587440686299746</v>
       </c>
-    </row>
-    <row r="12" spans="1:25">
+      <c r="Z11">
+        <v>0.4614979531594629</v>
+      </c>
+      <c r="AA11">
+        <v>0.3571413378316193</v>
+      </c>
+      <c r="AB11">
+        <v>0.1003758418828552</v>
+      </c>
+      <c r="AC11">
+        <v>0.387386645520173</v>
+      </c>
+      <c r="AD11">
+        <v>0.1410111613245825</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -3831,8 +4946,23 @@
       <c r="Y12">
         <v>0.0857931806852435</v>
       </c>
-    </row>
-    <row r="13" spans="1:25">
+      <c r="Z12">
+        <v>0.09459559446824144</v>
+      </c>
+      <c r="AA12">
+        <v>0.08665156808594135</v>
+      </c>
+      <c r="AB12">
+        <v>0.004604320567729011</v>
+      </c>
+      <c r="AC12">
+        <v>0.05453936271584398</v>
+      </c>
+      <c r="AD12">
+        <v>0.01585903243355465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -3908,8 +5038,23 @@
       <c r="Y13">
         <v>0.4763123189427804</v>
       </c>
-    </row>
-    <row r="14" spans="1:25">
+      <c r="Z13">
+        <v>0.288501753095905</v>
+      </c>
+      <c r="AA13">
+        <v>0.2392872642393567</v>
+      </c>
+      <c r="AB13">
+        <v>0.08054942350874707</v>
+      </c>
+      <c r="AC13">
+        <v>0.2433959641468699</v>
+      </c>
+      <c r="AD13">
+        <v>0.1115370820722504</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -3985,8 +5130,23 @@
       <c r="Y14">
         <v>0.3946932145079786</v>
       </c>
-    </row>
-    <row r="15" spans="1:25">
+      <c r="Z14">
+        <v>0.2940007019897914</v>
+      </c>
+      <c r="AA14">
+        <v>0.2277801628323287</v>
+      </c>
+      <c r="AB14">
+        <v>0.07857655733776951</v>
+      </c>
+      <c r="AC14">
+        <v>0.2401695322292717</v>
+      </c>
+      <c r="AD14">
+        <v>0.1008797501555453</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -4062,8 +5222,23 @@
       <c r="Y15">
         <v>0.1235921231630844</v>
       </c>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="Z15">
+        <v>0.2266471121656397</v>
+      </c>
+      <c r="AA15">
+        <v>0.08519098031865982</v>
+      </c>
+      <c r="AB15">
+        <v>0.08330546964629836</v>
+      </c>
+      <c r="AC15">
+        <v>0.1222791392523249</v>
+      </c>
+      <c r="AD15">
+        <v>0.02637061581093219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -4139,8 +5314,23 @@
       <c r="Y16">
         <v>0.4429816773248891</v>
       </c>
-    </row>
-    <row r="17" spans="1:25">
+      <c r="Z16">
+        <v>0.2339078539403656</v>
+      </c>
+      <c r="AA16">
+        <v>0.1794262784301446</v>
+      </c>
+      <c r="AB16">
+        <v>0.07784553391222809</v>
+      </c>
+      <c r="AC16">
+        <v>0.2441951714126266</v>
+      </c>
+      <c r="AD16">
+        <v>0.07969365107609198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -4216,8 +5406,23 @@
       <c r="Y17">
         <v>0.0547146395778307</v>
       </c>
-    </row>
-    <row r="18" spans="1:25">
+      <c r="Z17">
+        <v>0.07978131337933156</v>
+      </c>
+      <c r="AA17">
+        <v>0.08398505107803457</v>
+      </c>
+      <c r="AB17">
+        <v>0.02204578592569907</v>
+      </c>
+      <c r="AC17">
+        <v>0.1188509020803748</v>
+      </c>
+      <c r="AD17">
+        <v>0.06891785051191082</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -4293,8 +5498,23 @@
       <c r="Y18">
         <v>0.1417623644910922</v>
       </c>
-    </row>
-    <row r="19" spans="1:25">
+      <c r="Z18">
+        <v>0.1090067179111732</v>
+      </c>
+      <c r="AA18">
+        <v>0.153259485362287</v>
+      </c>
+      <c r="AB18">
+        <v>0.07734051915903606</v>
+      </c>
+      <c r="AC18">
+        <v>0.2309547356787035</v>
+      </c>
+      <c r="AD18">
+        <v>0.09066858794076781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -4370,8 +5590,23 @@
       <c r="Y19">
         <v>0.1134156476318669</v>
       </c>
-    </row>
-    <row r="20" spans="1:25">
+      <c r="Z19">
+        <v>0.1042602153685617</v>
+      </c>
+      <c r="AA19">
+        <v>0.1040008548923767</v>
+      </c>
+      <c r="AB19">
+        <v>0.01833751185327101</v>
+      </c>
+      <c r="AC19">
+        <v>0.1479497325712913</v>
+      </c>
+      <c r="AD19">
+        <v>0.05253189404050534</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -4447,8 +5682,23 @@
       <c r="Y20">
         <v>0.1439372892983369</v>
       </c>
-    </row>
-    <row r="21" spans="1:25">
+      <c r="Z20">
+        <v>0.09451123533496034</v>
+      </c>
+      <c r="AA20">
+        <v>0.09824837398228556</v>
+      </c>
+      <c r="AB20">
+        <v>0.03647835293774286</v>
+      </c>
+      <c r="AC20">
+        <v>0.1298248368729485</v>
+      </c>
+      <c r="AD20">
+        <v>0.0862994558227856</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -4524,8 +5774,23 @@
       <c r="Y21">
         <v>0.3615021366925845</v>
       </c>
-    </row>
-    <row r="22" spans="1:25">
+      <c r="Z21">
+        <v>0.2547515606633224</v>
+      </c>
+      <c r="AA21">
+        <v>0.1858343922485254</v>
+      </c>
+      <c r="AB21">
+        <v>0.05541252006931905</v>
+      </c>
+      <c r="AC21">
+        <v>0.2175123317038397</v>
+      </c>
+      <c r="AD21">
+        <v>0.05349579532179782</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -4601,8 +5866,23 @@
       <c r="Y22">
         <v>0.05235143600640564</v>
       </c>
-    </row>
-    <row r="23" spans="1:25">
+      <c r="Z22">
+        <v>0.07848660888741603</v>
+      </c>
+      <c r="AA22">
+        <v>0.09773796282031538</v>
+      </c>
+      <c r="AB22">
+        <v>0.04798702783296668</v>
+      </c>
+      <c r="AC22">
+        <v>0.1008692636441373</v>
+      </c>
+      <c r="AD22">
+        <v>0.03589898570568445</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -4678,8 +5958,23 @@
       <c r="Y23">
         <v>0.08970871183050549</v>
       </c>
-    </row>
-    <row r="24" spans="1:25">
+      <c r="Z23">
+        <v>0.1544181212519564</v>
+      </c>
+      <c r="AA23">
+        <v>0.1083892769266363</v>
+      </c>
+      <c r="AB23">
+        <v>0.04825139370953879</v>
+      </c>
+      <c r="AC23">
+        <v>0.1190822569680875</v>
+      </c>
+      <c r="AD23">
+        <v>0.07672412733656156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -4755,8 +6050,23 @@
       <c r="Y24">
         <v>0.07796063319020072</v>
       </c>
-    </row>
-    <row r="25" spans="1:25">
+      <c r="Z24">
+        <v>0.05448169925492293</v>
+      </c>
+      <c r="AA24">
+        <v>0.08332433801925829</v>
+      </c>
+      <c r="AB24">
+        <v>0.04012449923217935</v>
+      </c>
+      <c r="AC24">
+        <v>0.1620525835804314</v>
+      </c>
+      <c r="AD24">
+        <v>0.05063675627773986</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -4830,6 +6140,481 @@
         <v>0.07796063319020072</v>
       </c>
       <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>0.3599696426224733</v>
+      </c>
+      <c r="AA25">
+        <v>0.3053950438894737</v>
+      </c>
+      <c r="AB25">
+        <v>0.09874067094862374</v>
+      </c>
+      <c r="AC25">
+        <v>0.3587302793536627</v>
+      </c>
+      <c r="AD25">
+        <v>0.1012727170881194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>0.3700095530544901</v>
+      </c>
+      <c r="C26">
+        <v>0.8087384417639576</v>
+      </c>
+      <c r="D26">
+        <v>-0.8407884033512402</v>
+      </c>
+      <c r="E26">
+        <v>0.8553652132840053</v>
+      </c>
+      <c r="F26">
+        <v>0.8271192801682246</v>
+      </c>
+      <c r="G26">
+        <v>0.1507217195110394</v>
+      </c>
+      <c r="H26">
+        <v>0.5985886114067224</v>
+      </c>
+      <c r="I26">
+        <v>0.3411515208744616</v>
+      </c>
+      <c r="J26">
+        <v>-0.8407884033512402</v>
+      </c>
+      <c r="K26">
+        <v>0.4614979531594629</v>
+      </c>
+      <c r="L26">
+        <v>0.09459559446824144</v>
+      </c>
+      <c r="M26">
+        <v>0.288501753095905</v>
+      </c>
+      <c r="N26">
+        <v>0.2940007019897914</v>
+      </c>
+      <c r="O26">
+        <v>0.2266471121656397</v>
+      </c>
+      <c r="P26">
+        <v>0.2339078539403656</v>
+      </c>
+      <c r="Q26">
+        <v>0.07978131337933156</v>
+      </c>
+      <c r="R26">
+        <v>0.1090067179111732</v>
+      </c>
+      <c r="S26">
+        <v>0.1042602153685617</v>
+      </c>
+      <c r="T26">
+        <v>0.09451123533496034</v>
+      </c>
+      <c r="U26">
+        <v>0.2547515606633224</v>
+      </c>
+      <c r="V26">
+        <v>0.07848660888741603</v>
+      </c>
+      <c r="W26">
+        <v>0.1544181212519564</v>
+      </c>
+      <c r="X26">
+        <v>0.05448169925492293</v>
+      </c>
+      <c r="Y26">
+        <v>0.3599696426224733</v>
+      </c>
+      <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AA26">
+        <v>0.5644908993146162</v>
+      </c>
+      <c r="AB26">
+        <v>0.1155850257927707</v>
+      </c>
+      <c r="AC26">
+        <v>0.2887237163630078</v>
+      </c>
+      <c r="AD26">
+        <v>0.0968850911657775</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>0.1254003768781572</v>
+      </c>
+      <c r="C27">
+        <v>0.08182246775480589</v>
+      </c>
+      <c r="D27">
+        <v>-0.02977091124346888</v>
+      </c>
+      <c r="E27">
+        <v>0.3321391598127916</v>
+      </c>
+      <c r="F27">
+        <v>0.08667869488723651</v>
+      </c>
+      <c r="G27">
+        <v>0.1881029361635364</v>
+      </c>
+      <c r="H27">
+        <v>0.1876200439702971</v>
+      </c>
+      <c r="I27">
+        <v>0.2625775400123104</v>
+      </c>
+      <c r="J27">
+        <v>-0.02977091124346888</v>
+      </c>
+      <c r="K27">
+        <v>0.3571413378316193</v>
+      </c>
+      <c r="L27">
+        <v>0.08665156808594135</v>
+      </c>
+      <c r="M27">
+        <v>0.2392872642393567</v>
+      </c>
+      <c r="N27">
+        <v>0.2277801628323287</v>
+      </c>
+      <c r="O27">
+        <v>0.08519098031865982</v>
+      </c>
+      <c r="P27">
+        <v>0.1794262784301446</v>
+      </c>
+      <c r="Q27">
+        <v>0.08398505107803457</v>
+      </c>
+      <c r="R27">
+        <v>0.153259485362287</v>
+      </c>
+      <c r="S27">
+        <v>0.1040008548923767</v>
+      </c>
+      <c r="T27">
+        <v>0.09824837398228556</v>
+      </c>
+      <c r="U27">
+        <v>0.1858343922485254</v>
+      </c>
+      <c r="V27">
+        <v>0.09773796282031538</v>
+      </c>
+      <c r="W27">
+        <v>0.1083892769266363</v>
+      </c>
+      <c r="X27">
+        <v>0.08332433801925829</v>
+      </c>
+      <c r="Y27">
+        <v>0.3053950438894737</v>
+      </c>
+      <c r="Z27">
+        <v>0.5644908993146162</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <v>0.1455054548865966</v>
+      </c>
+      <c r="AC27">
+        <v>0.5384510741843077</v>
+      </c>
+      <c r="AD27">
+        <v>0.1776205629263073</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>0.09362397374024603</v>
+      </c>
+      <c r="C28">
+        <v>0.4140484508790929</v>
+      </c>
+      <c r="D28">
+        <v>-0.0455033566070495</v>
+      </c>
+      <c r="E28">
+        <v>0.1448423863224391</v>
+      </c>
+      <c r="F28">
+        <v>0.0785868806609568</v>
+      </c>
+      <c r="G28">
+        <v>0.05060933887733886</v>
+      </c>
+      <c r="H28">
+        <v>0.06628412924595636</v>
+      </c>
+      <c r="I28">
+        <v>0.05655167039615811</v>
+      </c>
+      <c r="J28">
+        <v>-0.0455033566070495</v>
+      </c>
+      <c r="K28">
+        <v>0.1003758418828552</v>
+      </c>
+      <c r="L28">
+        <v>0.004604320567729011</v>
+      </c>
+      <c r="M28">
+        <v>0.08054942350874707</v>
+      </c>
+      <c r="N28">
+        <v>0.07857655733776951</v>
+      </c>
+      <c r="O28">
+        <v>0.08330546964629836</v>
+      </c>
+      <c r="P28">
+        <v>0.07784553391222809</v>
+      </c>
+      <c r="Q28">
+        <v>0.02204578592569907</v>
+      </c>
+      <c r="R28">
+        <v>0.07734051915903606</v>
+      </c>
+      <c r="S28">
+        <v>0.01833751185327101</v>
+      </c>
+      <c r="T28">
+        <v>0.03647835293774286</v>
+      </c>
+      <c r="U28">
+        <v>0.05541252006931905</v>
+      </c>
+      <c r="V28">
+        <v>0.04798702783296668</v>
+      </c>
+      <c r="W28">
+        <v>0.04825139370953879</v>
+      </c>
+      <c r="X28">
+        <v>0.04012449923217935</v>
+      </c>
+      <c r="Y28">
+        <v>0.09874067094862374</v>
+      </c>
+      <c r="Z28">
+        <v>0.1155850257927707</v>
+      </c>
+      <c r="AA28">
+        <v>0.1455054548865966</v>
+      </c>
+      <c r="AB28">
+        <v>1</v>
+      </c>
+      <c r="AC28">
+        <v>0.1862798874323739</v>
+      </c>
+      <c r="AD28">
+        <v>0.1107768734496421</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0.1723215232906715</v>
+      </c>
+      <c r="C29">
+        <v>0.06387138136257922</v>
+      </c>
+      <c r="D29">
+        <v>0.006492231348953815</v>
+      </c>
+      <c r="E29">
+        <v>0.5692315229931343</v>
+      </c>
+      <c r="F29">
+        <v>0.06429824212392583</v>
+      </c>
+      <c r="G29">
+        <v>0.2058852927497622</v>
+      </c>
+      <c r="H29">
+        <v>0.2171265467651519</v>
+      </c>
+      <c r="I29">
+        <v>0.2408767397452142</v>
+      </c>
+      <c r="J29">
+        <v>0.006492231348953815</v>
+      </c>
+      <c r="K29">
+        <v>0.387386645520173</v>
+      </c>
+      <c r="L29">
+        <v>0.05453936271584398</v>
+      </c>
+      <c r="M29">
+        <v>0.2433959641468699</v>
+      </c>
+      <c r="N29">
+        <v>0.2401695322292717</v>
+      </c>
+      <c r="O29">
+        <v>0.1222791392523249</v>
+      </c>
+      <c r="P29">
+        <v>0.2441951714126266</v>
+      </c>
+      <c r="Q29">
+        <v>0.1188509020803748</v>
+      </c>
+      <c r="R29">
+        <v>0.2309547356787035</v>
+      </c>
+      <c r="S29">
+        <v>0.1479497325712913</v>
+      </c>
+      <c r="T29">
+        <v>0.1298248368729485</v>
+      </c>
+      <c r="U29">
+        <v>0.2175123317038397</v>
+      </c>
+      <c r="V29">
+        <v>0.1008692636441373</v>
+      </c>
+      <c r="W29">
+        <v>0.1190822569680875</v>
+      </c>
+      <c r="X29">
+        <v>0.1620525835804314</v>
+      </c>
+      <c r="Y29">
+        <v>0.3587302793536627</v>
+      </c>
+      <c r="Z29">
+        <v>0.2887237163630078</v>
+      </c>
+      <c r="AA29">
+        <v>0.5384510741843077</v>
+      </c>
+      <c r="AB29">
+        <v>0.1862798874323739</v>
+      </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
+      <c r="AD29">
+        <v>0.2051048790416753</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>0.0631335134076476</v>
+      </c>
+      <c r="C30">
+        <v>0.04216446582810775</v>
+      </c>
+      <c r="D30">
+        <v>-0.0006806693777868312</v>
+      </c>
+      <c r="E30">
+        <v>0.1215881699463247</v>
+      </c>
+      <c r="F30">
+        <v>0.3059705690643176</v>
+      </c>
+      <c r="G30">
+        <v>0.09016094561642715</v>
+      </c>
+      <c r="H30">
+        <v>0.0991097596899662</v>
+      </c>
+      <c r="I30">
+        <v>0.1054463576487062</v>
+      </c>
+      <c r="J30">
+        <v>-0.0006806693777868312</v>
+      </c>
+      <c r="K30">
+        <v>0.1410111613245825</v>
+      </c>
+      <c r="L30">
+        <v>0.01585903243355465</v>
+      </c>
+      <c r="M30">
+        <v>0.1115370820722504</v>
+      </c>
+      <c r="N30">
+        <v>0.1008797501555453</v>
+      </c>
+      <c r="O30">
+        <v>0.02637061581093219</v>
+      </c>
+      <c r="P30">
+        <v>0.07969365107609198</v>
+      </c>
+      <c r="Q30">
+        <v>0.06891785051191082</v>
+      </c>
+      <c r="R30">
+        <v>0.09066858794076781</v>
+      </c>
+      <c r="S30">
+        <v>0.05253189404050534</v>
+      </c>
+      <c r="T30">
+        <v>0.0862994558227856</v>
+      </c>
+      <c r="U30">
+        <v>0.05349579532179782</v>
+      </c>
+      <c r="V30">
+        <v>0.03589898570568445</v>
+      </c>
+      <c r="W30">
+        <v>0.07672412733656156</v>
+      </c>
+      <c r="X30">
+        <v>0.05063675627773986</v>
+      </c>
+      <c r="Y30">
+        <v>0.1012727170881194</v>
+      </c>
+      <c r="Z30">
+        <v>0.0968850911657775</v>
+      </c>
+      <c r="AA30">
+        <v>0.1776205629263073</v>
+      </c>
+      <c r="AB30">
+        <v>0.1107768734496421</v>
+      </c>
+      <c r="AC30">
+        <v>0.2051048790416753</v>
+      </c>
+      <c r="AD30">
         <v>1</v>
       </c>
     </row>

</xml_diff>